<commit_message>
archivo de contacto de prueba
</commit_message>
<xml_diff>
--- a/contacts.xlsx
+++ b/contacts.xlsx
@@ -20,9 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t xml:space="preserve">Francisco Sannet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hola</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H</t>
   </si>
 </sst>
 </file>
@@ -120,10 +126,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -136,6 +142,16 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
funciones para obtener ultimo mensaje de whatsapp y la hora en el que fue enviado
</commit_message>
<xml_diff>
--- a/contacts.xlsx
+++ b/contacts.xlsx
@@ -20,15 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t xml:space="preserve">Francisco Sannet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hola</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H</t>
+    <t xml:space="preserve">Julio César Pérez</t>
   </si>
 </sst>
 </file>
@@ -126,10 +120,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -142,16 +136,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>2</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>